<commit_message>
Entrego algoritmos que retornan listas de escalares
</commit_message>
<xml_diff>
--- a/Especificaciones.xlsx
+++ b/Especificaciones.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orct\Documents\Visual Studio 2015\Projects\SM.VB.DiseñoConPruebasUnitarias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orct\Source\Repos\sm.vb.diseno-con-pruebas-unitarias\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13875" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13875" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="introducción" sheetId="6" r:id="rId1"/>
-    <sheet name="escalar" sheetId="1" r:id="rId2"/>
-    <sheet name="validacion" sheetId="2" r:id="rId3"/>
-    <sheet name="lista de escalares" sheetId="3" r:id="rId4"/>
-    <sheet name="estructura de datos" sheetId="4" r:id="rId5"/>
-    <sheet name="lista de estructuras de datos" sheetId="5" r:id="rId6"/>
+    <sheet name="Introducción" sheetId="6" r:id="rId1"/>
+    <sheet name="Cómo programarlo" sheetId="7" r:id="rId2"/>
+    <sheet name="escalar" sheetId="1" r:id="rId3"/>
+    <sheet name="validacion" sheetId="2" r:id="rId4"/>
+    <sheet name="lista de escalares" sheetId="3" r:id="rId5"/>
+    <sheet name="estructura de datos" sheetId="4" r:id="rId6"/>
+    <sheet name="lista de estructuras de datos" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -71,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A34" authorId="0" shapeId="0">
+    <comment ref="A35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A35" authorId="0" shapeId="0">
+    <comment ref="A36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B69" authorId="0" shapeId="0">
+    <comment ref="B72" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -110,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B83" authorId="0" shapeId="0">
+    <comment ref="B86" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -123,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A93" authorId="0" shapeId="0">
+    <comment ref="A96" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -185,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B28" authorId="0" shapeId="0">
+    <comment ref="C28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -200,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C28" authorId="0" shapeId="0">
+    <comment ref="D28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -213,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D28" authorId="0" shapeId="0">
+    <comment ref="E28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -227,7 +228,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E28" authorId="0" shapeId="0">
+    <comment ref="F28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -253,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D38" authorId="0" shapeId="0">
+    <comment ref="E39" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -266,7 +267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E39" authorId="0" shapeId="0">
+    <comment ref="F40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -279,7 +280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E59" authorId="0" shapeId="0">
+    <comment ref="E60" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -316,7 +317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="0" shapeId="0">
+    <comment ref="A19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -327,6 +328,19 @@
           </rPr>
           <t>Al retornar una lista, se asume que el algoritmo que retorna un escalar tiene sus pruebas unitarias.
 Aquí no es necesario revisar todos los casos.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B27" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Cero significa que la historia no está terminada</t>
         </r>
       </text>
     </comment>
@@ -567,7 +581,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="255">
   <si>
     <t>Genere la métrica de puntos</t>
   </si>
@@ -632,9 +646,6 @@
     <t>Podría no haber información disponible</t>
   </si>
   <si>
-    <t>Modifique la métrica de puntos de acuerdo a la siguiente tabla</t>
-  </si>
-  <si>
     <t>89% 9.5|8.5</t>
   </si>
   <si>
@@ -659,9 +670,6 @@
     <t>Hay informacion de dias disponible</t>
   </si>
   <si>
-    <t>Métrica de tiempo no efectivo</t>
-  </si>
-  <si>
     <t>Se redondea a un decimal</t>
   </si>
   <si>
@@ -776,18 +784,9 @@
     <t>Algoritmos que retornan una lista de escalares</t>
   </si>
   <si>
-    <t>Genere la lista de métricas de puntos</t>
-  </si>
-  <si>
     <t>Dadas</t>
   </si>
   <si>
-    <t>se genera las métricas para iteraciones con estos datos</t>
-  </si>
-  <si>
-    <t>se obtiene la lista siguiente</t>
-  </si>
-  <si>
     <t xml:space="preserve">Recomendación: </t>
   </si>
   <si>
@@ -797,33 +796,15 @@
     <t xml:space="preserve">Cuando </t>
   </si>
   <si>
-    <t>se genera la velocidad para cada iteración de acuerdo a las siguientes historias</t>
-  </si>
-  <si>
     <t>Historia terminada en iteración</t>
   </si>
   <si>
     <t>Puntos de la historia</t>
   </si>
   <si>
-    <t>Genere la lista de métricas de velocidad por iteración de acuerdo a las historias.</t>
-  </si>
-  <si>
     <t>Especifique una regla de negocio que obtenga la velocidad para una iteración dada (ej. Dadas las iteraciones, cuál es la velocidad para la iteración #1?)</t>
   </si>
   <si>
-    <t>"95%", "91%", "89%"</t>
-  </si>
-  <si>
-    <t>las iteraciones siguientes: 1,2,3</t>
-  </si>
-  <si>
-    <t>la lista de velocidades por iteración es 11, 2, 5</t>
-  </si>
-  <si>
-    <t>Genere la métrica de velocidad para una iteración de acuerdo a las historias terminadas en la misma.</t>
-  </si>
-  <si>
     <t>Utilice la regla de negocio que obtiene la velocidad para una iteración dada.</t>
   </si>
   <si>
@@ -1260,6 +1241,111 @@
   </si>
   <si>
     <t>Tiempo no efectivo debe ser igual o menor a la Capacidad del equipo</t>
+  </si>
+  <si>
+    <t>Terminada en iteración</t>
+  </si>
+  <si>
+    <t>Ejercicio: utilice la clase Iteracion con las tres propiedades nuevas.</t>
+  </si>
+  <si>
+    <t>Genere la métrica de velocidad para una iteración</t>
+  </si>
+  <si>
+    <t>Modifique la métrica de puntos</t>
+  </si>
+  <si>
+    <t>Si no hay informacion de puntos disponible no se validan</t>
+  </si>
+  <si>
+    <t>Ejercicio: Utilice una clase "Iteracion" con tres propiedades.</t>
+  </si>
+  <si>
+    <t>Ejercicio: Utilice una clase "Iteracion"</t>
+  </si>
+  <si>
+    <t>las siguientes historias</t>
+  </si>
+  <si>
+    <t>se genera las velocidades para las iteraciones 1,2,3</t>
+  </si>
+  <si>
+    <t>Utilice la regla de negocio que obtiene la métrica para una sola iteración.</t>
+  </si>
+  <si>
+    <t>Genere la lista de métricas de puntos.</t>
+  </si>
+  <si>
+    <t>Genere la lista de métricas de velocidad.</t>
+  </si>
+  <si>
+    <t>Parametros y sus tipos</t>
+  </si>
+  <si>
+    <t>Salidas y sus tipos</t>
+  </si>
+  <si>
+    <t>El resultado esperado</t>
+  </si>
+  <si>
+    <t>La inicializacion de parametros y la asignacion del resultado obtenido</t>
+  </si>
+  <si>
+    <t>La comparación por realizar.</t>
+  </si>
+  <si>
+    <t>2. Determine la firma del metodo por programar:</t>
+  </si>
+  <si>
+    <t>3. Cree la clase de pruebas unitarias, en una estructura de folders igual al codigo por probar</t>
+  </si>
+  <si>
+    <t>4. Cree el primer metodo de pruebas unitarias, con el primer ejemplo, indicando:</t>
+  </si>
+  <si>
+    <t>5. Ejecute mirando que el codigo compile pero que la prueba falle.</t>
+  </si>
+  <si>
+    <t>6. Escriba el codigo que razonablemente haga que la prueba pase.</t>
+  </si>
+  <si>
+    <t>7. Repita sucesivamente para cada ejemplo, mirando que todas las pruebas anteriores sigan funcionando.</t>
+  </si>
+  <si>
+    <t>Nombre: un nombre imperativo que explique el algoritmo</t>
+  </si>
+  <si>
+    <t>1. Lea el ejemplo. Aclare conceptos y tipos de datos. Busque que los casos límite tengan un ejemplo.</t>
+  </si>
+  <si>
+    <t>la lista de velocidades por iteración obtenida es 8, 10, 1</t>
+  </si>
+  <si>
+    <t>Recomendaciones</t>
+  </si>
+  <si>
+    <t>Inicie a programar solamente cuando entienda muy bien el ejemplo y sus conceptos.</t>
+  </si>
+  <si>
+    <t>Programe un ejemplo a la vez.</t>
+  </si>
+  <si>
+    <t>Siempre vea que la prueba falle antes de intentar hacerla exitosa.</t>
+  </si>
+  <si>
+    <t>Métricas de puntos</t>
+  </si>
+  <si>
+    <t>se genera las métricas para las iteraciones</t>
+  </si>
+  <si>
+    <t>Cada fila corresponde a una iteración</t>
+  </si>
+  <si>
+    <t>las métricas de puntos son</t>
+  </si>
+  <si>
+    <t>Pasos para programar una especificación con ejemplos</t>
   </si>
 </sst>
 </file>
@@ -1270,7 +1356,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1357,6 +1443,12 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1470,7 +1562,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1509,6 +1601,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="8" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="7"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1" xfId="8" builtinId="30"/>
@@ -1523,7 +1621,101 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="7" builtinId="10"/>
   </cellStyles>
-  <dxfs count="51">
+  <dxfs count="56">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
@@ -2322,8 +2514,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="50"/>
-      <tableStyleElement type="headerRow" dxfId="49"/>
+      <tableStyleElement type="wholeTable" dxfId="55"/>
+      <tableStyleElement type="headerRow" dxfId="54"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -2351,12 +2543,12 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Table28" displayName="Table28" ref="A22:C23" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Table28" displayName="Table28" ref="A22:C23" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
   <autoFilter ref="A22:C23"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Monto nominal del saldo" dataDxfId="27" dataCellStyle="Comma"/>
-    <tableColumn id="2" name="Precio limpio del vector de precios" dataDxfId="26"/>
-    <tableColumn id="3" name="Valor de mercado" dataDxfId="25" dataCellStyle="Comma">
+    <tableColumn id="1" name="Monto nominal del saldo" dataDxfId="32" dataCellStyle="Comma"/>
+    <tableColumn id="2" name="Precio limpio del vector de precios" dataDxfId="31"/>
+    <tableColumn id="3" name="Valor de mercado" dataDxfId="30" dataCellStyle="Comma">
       <calculatedColumnFormula>+Table28[Monto nominal del saldo]*(Table28[Precio limpio del vector de precios]/100)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2365,14 +2557,14 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Table2830" displayName="Table2830" ref="A28:C29" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Table2830" displayName="Table2830" ref="A28:C29" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="A28:C29"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Valor de mercado" dataDxfId="21" dataCellStyle="Comma">
+    <tableColumn id="1" name="Valor de mercado" dataDxfId="26" dataCellStyle="Comma">
       <calculatedColumnFormula>+Table28[Monto nominal del saldo]*(Table28[Precio limpio del vector de precios]/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Porcentaje de cobertura revisado" dataDxfId="20"/>
-    <tableColumn id="3" name="Aporte de garantía" dataDxfId="19" dataCellStyle="Comma">
+    <tableColumn id="2" name="Porcentaje de cobertura revisado" dataDxfId="25"/>
+    <tableColumn id="3" name="Aporte de garantía" dataDxfId="24" dataCellStyle="Comma">
       <calculatedColumnFormula>+Table2830[Valor de mercado]*Table2830[Porcentaje de cobertura revisado]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2384,7 +2576,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="A15:E19" totalsRowShown="0">
   <autoFilter ref="A15:E19"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="18"/>
+    <tableColumn id="1" name="Ejemplo" dataDxfId="23"/>
     <tableColumn id="2" name="Numero"/>
     <tableColumn id="3" name="Fecha inicial"/>
     <tableColumn id="4" name="Fecha final"/>
@@ -2398,58 +2590,59 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B6:C8" totalsRowShown="0">
   <autoFilter ref="B6:C8"/>
   <tableColumns count="2">
-    <tableColumn id="2" name="Fecha de inicio" dataDxfId="17"/>
-    <tableColumn id="3" name="Fecha final" dataDxfId="16"/>
+    <tableColumn id="2" name="Fecha de inicio" dataDxfId="22"/>
+    <tableColumn id="3" name="Fecha final" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table168" displayName="Table168" ref="A28:F45" totalsRowShown="0">
-  <autoFilter ref="A28:F45"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table168" displayName="Table168" ref="A28:G46" totalsRowShown="0">
+  <autoFilter ref="A28:G46"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Ejemplo" dataDxfId="20"/>
+    <tableColumn id="7" name="Hay informacion de puntos disponible" dataDxfId="4"/>
     <tableColumn id="2" name="Puntos planificados" dataCellStyle="Normal"/>
     <tableColumn id="3" name="Puntos terminados" dataCellStyle="Normal"/>
     <tableColumn id="4" name="Capacidad del equipo" dataCellStyle="Normal"/>
     <tableColumn id="5" name="Tiempo no efectivo"/>
-    <tableColumn id="6" name="Es válida o no" dataDxfId="14"/>
+    <tableColumn id="6" name="Es válida o no" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1689" displayName="Table1689" ref="A55:F61" totalsRowShown="0">
-  <autoFilter ref="A55:F61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1689" displayName="Table1689" ref="A56:F62" totalsRowShown="0">
+  <autoFilter ref="A56:F62"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="13"/>
-    <tableColumn id="7" name="Fecha actual" dataDxfId="12"/>
+    <tableColumn id="1" name="Ejemplo" dataDxfId="18"/>
+    <tableColumn id="7" name="Fecha actual" dataDxfId="17"/>
     <tableColumn id="2" name="Fecha de reporte" dataCellStyle="Normal"/>
     <tableColumn id="3" name="Total de incidentes" dataCellStyle="Normal"/>
     <tableColumn id="4" name="Descripción" dataCellStyle="Normal"/>
-    <tableColumn id="6" name="Es válida o no" dataDxfId="11"/>
+    <tableColumn id="6" name="Es válida o no" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="B8:D11" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="B8:D11" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
   <autoFilter ref="B8:D11"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Puntos planificados" dataDxfId="7"/>
-    <tableColumn id="2" name="Puntos terminados" dataDxfId="6"/>
-    <tableColumn id="3" name="Hay informacion de puntos disponible" dataDxfId="5"/>
+    <tableColumn id="1" name="Puntos planificados" dataDxfId="12"/>
+    <tableColumn id="2" name="Puntos terminados" dataDxfId="11"/>
+    <tableColumn id="3" name="Hay informacion de puntos disponible" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="B22:C29" totalsRowShown="0">
-  <autoFilter ref="B22:C29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="B24:C31" totalsRowShown="0">
+  <autoFilter ref="B24:C31"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Historia terminada en iteración"/>
     <tableColumn id="2" name="Puntos de la historia"/>
@@ -2459,6 +2652,16 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table5" displayName="Table5" ref="B14:B17" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="3">
+  <autoFilter ref="B14:B17"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Métricas de puntos" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table3" displayName="Table3" ref="A7:D16" totalsRowShown="0">
   <autoFilter ref="A7:D16"/>
   <tableColumns count="4">
@@ -2471,12 +2674,23 @@
 </table>
 </file>
 
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table17" displayName="Table17" ref="C57:D64" totalsRowShown="0">
+  <autoFilter ref="C57:D64"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Historia terminada en iteración" dataDxfId="53"/>
+    <tableColumn id="2" name="Puntos de la historia" dataDxfId="52"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table412" displayName="Table412" ref="A21:D22" totalsRowShown="0">
   <autoFilter ref="A21:D22"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Iteración"/>
-    <tableColumn id="2" name="puntos en el alcance" dataDxfId="4"/>
+    <tableColumn id="2" name="puntos en el alcance" dataDxfId="9"/>
     <tableColumn id="3" name="velocidad"/>
     <tableColumn id="4" name="puntos terminados acumulados"/>
   </tableColumns>
@@ -2484,18 +2698,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table17" displayName="Table17" ref="C57:D64" totalsRowShown="0">
-  <autoFilter ref="C57:D64"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Historia terminada en iteración" dataDxfId="48"/>
-    <tableColumn id="2" name="Puntos de la historia" dataDxfId="47"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table1021" displayName="Table1021" ref="A33:B36" totalsRowShown="0">
   <autoFilter ref="A33:B36"/>
   <tableColumns count="2">
@@ -2506,7 +2709,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Table24" displayName="Table24" ref="B53:E54" totalsRowShown="0">
   <autoFilter ref="B53:E54"/>
   <tableColumns count="4">
@@ -2519,11 +2722,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Table25" displayName="Table25" ref="B45:E46" totalsRowShown="0">
   <autoFilter ref="B45:E46"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="3"/>
+    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="8"/>
     <tableColumn id="2" name="Dias minimos al vencimiento del emisor"/>
     <tableColumn id="3" name="Porcentaje de cobertura"/>
     <tableColumn id="4" name="Precio limpio del vector de precios"/>
@@ -2532,7 +2735,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Table26" displayName="Table26" ref="B49:C50" totalsRowShown="0">
   <autoFilter ref="B49:C50"/>
   <tableColumns count="2">
@@ -2543,7 +2746,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table323" displayName="Table323" ref="A6:D15" totalsRowShown="0">
   <autoFilter ref="A6:D15"/>
   <tableColumns count="4">
@@ -2556,12 +2759,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Table4" displayName="Table4" ref="A20:D24" totalsRowShown="0">
   <autoFilter ref="A20:D24"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Iteración"/>
-    <tableColumn id="2" name="puntos en el alcance" dataDxfId="2">
+    <tableColumn id="2" name="puntos en el alcance" dataDxfId="7">
       <calculatedColumnFormula>+A20+A21+A23+A24</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="velocidad"/>
@@ -2571,7 +2774,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Table2431" displayName="Table2431" ref="B43:E45" totalsRowShown="0">
   <autoFilter ref="B43:E45"/>
   <tableColumns count="4">
@@ -2584,12 +2787,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Table2532" displayName="Table2532" ref="B33:F35" totalsRowShown="0">
   <autoFilter ref="B33:F35"/>
   <tableColumns count="5">
-    <tableColumn id="5" name="ISIN" dataDxfId="1"/>
-    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="0"/>
+    <tableColumn id="5" name="ISIN" dataDxfId="6"/>
+    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="5"/>
     <tableColumn id="2" name="Dias minimos al vencimiento del emisor"/>
     <tableColumn id="3" name="Porcentaje de cobertura"/>
     <tableColumn id="4" name="Precio limpio del vector de precios"/>
@@ -2598,7 +2801,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="Table2633" displayName="Table2633" ref="B38:C40" totalsRowShown="0">
   <autoFilter ref="B38:C40"/>
   <tableColumns count="2">
@@ -2610,22 +2813,22 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table1118" displayName="Table1118" ref="B69:D72" totalsRowShown="0" headerRowDxfId="46" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table1118" displayName="Table1118" ref="B69:D72" totalsRowShown="0" headerRowDxfId="51" tableBorderDxfId="50">
   <autoFilter ref="B69:D72"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="44"/>
-    <tableColumn id="2" name="Iteración" dataDxfId="43"/>
-    <tableColumn id="3" name="Velocidad" dataDxfId="42"/>
+    <tableColumn id="1" name="Ejemplo" dataDxfId="49"/>
+    <tableColumn id="2" name="Iteración" dataDxfId="48"/>
+    <tableColumn id="3" name="Velocidad" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A39:E44" totalsRowShown="0">
-  <autoFilter ref="A39:E44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A40:E45" totalsRowShown="0">
+  <autoFilter ref="A40:E45"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="41"/>
+    <tableColumn id="1" name="Ejemplo" dataDxfId="46"/>
     <tableColumn id="2" name="Puntos planificados"/>
     <tableColumn id="3" name="Puntos terminados"/>
     <tableColumn id="4" name="Hay informacion de puntos disponible"/>
@@ -2636,10 +2839,10 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A54:E59" totalsRowShown="0">
-  <autoFilter ref="A54:E59"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A56:E61" totalsRowShown="0">
+  <autoFilter ref="A56:E61"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="40"/>
+    <tableColumn id="1" name="Ejemplo" dataDxfId="45"/>
     <tableColumn id="2" name="Puntos planificados"/>
     <tableColumn id="3" name="Puntos terminados"/>
     <tableColumn id="4" name="Hay informacion de puntos disponible"/>
@@ -2650,37 +2853,37 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A69:E73" totalsRowShown="0">
-  <autoFilter ref="A69:E73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A72:E76" totalsRowShown="0">
+  <autoFilter ref="A72:E76"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="39"/>
+    <tableColumn id="1" name="Ejemplo" dataDxfId="44"/>
     <tableColumn id="2" name="Capacidad del equipo"/>
     <tableColumn id="3" name="Dias no efectivos"/>
     <tableColumn id="4" name="Hay informacion de dias disponible"/>
-    <tableColumn id="5" name="Métrica de tiempo no efectivo"/>
+    <tableColumn id="5" name="Tiempo no efectivo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1210" displayName="Table1210" ref="B80:C87" totalsRowShown="0">
-  <autoFilter ref="B80:C87"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1210" displayName="Table1210" ref="B83:C90" totalsRowShown="0">
+  <autoFilter ref="B83:C90"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Historia terminada en iteración"/>
-    <tableColumn id="2" name="Puntos de la historia"/>
+    <tableColumn id="1" name="Terminada en iteración"/>
+    <tableColumn id="2" name="Puntos"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A92:C95" totalsRowShown="0" headerRowDxfId="38" tableBorderDxfId="37">
-  <autoFilter ref="A92:C95"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A95:C98" totalsRowShown="0" headerRowDxfId="43" tableBorderDxfId="42">
+  <autoFilter ref="A95:C98"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="36"/>
-    <tableColumn id="2" name="Iteración" dataDxfId="35"/>
-    <tableColumn id="3" name="Velocidad" dataDxfId="34"/>
+    <tableColumn id="1" name="Ejemplo" dataDxfId="41"/>
+    <tableColumn id="2" name="Iteración" dataDxfId="40"/>
+    <tableColumn id="3" name="Velocidad" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2690,9 +2893,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Table27" displayName="Table27" ref="A12:E15" totalsRowShown="0">
   <autoFilter ref="A12:E15"/>
   <tableColumns count="5">
-    <tableColumn id="5" name="Ejemplo" dataDxfId="33"/>
-    <tableColumn id="4" name="Fecha actual" dataDxfId="32"/>
-    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="31"/>
+    <tableColumn id="5" name="Ejemplo" dataDxfId="38"/>
+    <tableColumn id="4" name="Fecha actual" dataDxfId="37"/>
+    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="36"/>
     <tableColumn id="2" name="Dias minimos al vencimiento del emisor"/>
     <tableColumn id="3" name="Porcentaje de cobertura revisado"/>
   </tableColumns>
@@ -2965,8 +3168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2980,33 +3183,33 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3016,10 +3219,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
@@ -3031,7 +3234,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="H10" s="31"/>
       <c r="I10" s="31"/>
@@ -3044,10 +3247,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
@@ -3072,10 +3275,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="20" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
@@ -3100,7 +3303,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="H18" s="31"/>
       <c r="I18" s="31"/>
@@ -3116,7 +3319,7 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -3124,7 +3327,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -3132,37 +3335,37 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -3170,7 +3373,7 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3178,7 +3381,7 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3186,7 +3389,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3199,18 +3402,18 @@
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D38" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="E38" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C39">
         <v>1000</v>
@@ -3224,7 +3427,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C40">
         <v>1000</v>
@@ -3238,7 +3441,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C41">
         <v>1000</v>
@@ -3252,7 +3455,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C42">
         <v>1000</v>
@@ -3266,65 +3469,65 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B44" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="18" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B51" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C56" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
       <c r="C57" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D57" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3395,10 +3598,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C66" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3406,7 +3609,7 @@
         <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3414,15 +3617,15 @@
         <v>6</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B70" s="16" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C70">
         <v>4</v>
@@ -3433,7 +3636,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B71" s="16" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -3444,7 +3647,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B72" s="16" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C72">
         <v>2</v>
@@ -3455,40 +3658,40 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="23" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B74" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="24" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="24" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="24" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="24" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3507,12 +3710,124 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="96.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="38" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="38" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3520,29 +3835,29 @@
     <col min="2" max="2" width="36.5703125" customWidth="1"/>
     <col min="3" max="3" width="38.42578125" customWidth="1"/>
     <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3550,15 +3865,15 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B7" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3566,7 +3881,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3574,7 +3889,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3587,21 +3902,21 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D12" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="E12" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B13" s="9">
         <v>42370</v>
@@ -3618,7 +3933,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B14" s="9">
         <v>42370</v>
@@ -3635,7 +3950,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="B15" s="9">
         <v>42370</v>
@@ -3657,7 +3972,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B17" s="30"/>
       <c r="C17" s="9"/>
@@ -3669,16 +3984,16 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B19" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="C19" s="9"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -3690,13 +4005,13 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3718,16 +4033,16 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B25" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="C25" s="9"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -3739,13 +4054,13 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3768,470 +4083,458 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B31" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C31" s="32"/>
+      <c r="C31" s="36"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" t="s">
-        <v>54</v>
+    <row r="33" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>6</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>7</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>8</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>9</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E40" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B40">
-        <v>100</v>
-      </c>
-      <c r="C40">
-        <v>95</v>
-      </c>
-      <c r="D40" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="1">
-        <v>0.95</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B41">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C41">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
       </c>
       <c r="E41" s="1">
-        <v>0.91</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B42">
-        <v>9.5</v>
+        <v>99</v>
       </c>
       <c r="C42">
-        <v>8.5</v>
+        <v>90</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
       </c>
       <c r="E42" s="1">
-        <v>0.89</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="C43">
-        <v>10</v>
+        <v>8.5</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
       </c>
-      <c r="E43" t="s">
-        <v>15</v>
+      <c r="E43" s="1">
+        <v>0.89</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45">
         <v>0</v>
       </c>
-      <c r="D44" t="s">
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45" t="s">
         <v>13</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E45" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B46" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C46" s="32"/>
-    </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="C47" s="36"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-    </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B49" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B50" t="s">
-        <v>4</v>
+      <c r="B51" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>6</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B56" t="s">
         <v>7</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C56" t="s">
         <v>8</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D56" t="s">
         <v>9</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E56" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B55">
-        <v>100</v>
-      </c>
-      <c r="C55">
-        <v>95</v>
-      </c>
-      <c r="D55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B56">
-        <v>99</v>
-      </c>
-      <c r="C56">
-        <v>90</v>
-      </c>
-      <c r="D56" t="s">
-        <v>12</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B57">
-        <v>9.5</v>
+        <v>100</v>
       </c>
       <c r="C57">
-        <v>8.5</v>
+        <v>95</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>22</v>
+        <v>196</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="C58">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
       </c>
-      <c r="E58" t="s">
-        <v>23</v>
+      <c r="E58" s="1" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59">
+        <v>9.5</v>
+      </c>
+      <c r="C59">
+        <v>8.5</v>
+      </c>
+      <c r="D59" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>10</v>
+      </c>
+      <c r="D60" t="s">
+        <v>12</v>
+      </c>
+      <c r="E60" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B59">
+      <c r="B61">
         <v>0</v>
       </c>
-      <c r="C59">
+      <c r="C61">
         <v>0</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D61" t="s">
         <v>13</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E61" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B61" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
-        <v>24</v>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B63" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B64" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B65" t="s">
-        <v>25</v>
+      <c r="A64" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>6</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B72" t="s">
+        <v>26</v>
+      </c>
+      <c r="C72" t="s">
         <v>27</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D72" t="s">
         <v>28</v>
       </c>
-      <c r="D69" t="s">
-        <v>29</v>
-      </c>
-      <c r="E69" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B70">
-        <v>100</v>
-      </c>
-      <c r="C70">
-        <v>5</v>
-      </c>
-      <c r="D70" t="s">
-        <v>12</v>
-      </c>
-      <c r="E70" s="5">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B71">
-        <v>99</v>
-      </c>
-      <c r="C71">
-        <v>5.67</v>
-      </c>
-      <c r="D71" t="s">
-        <v>12</v>
-      </c>
-      <c r="E71" s="5">
-        <v>5.7000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B72">
-        <v>100</v>
-      </c>
-      <c r="C72">
-        <v>0</v>
-      </c>
-      <c r="D72" t="s">
-        <v>12</v>
-      </c>
-      <c r="E72" s="5">
-        <v>0</v>
+      <c r="E72" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B73">
+        <v>100</v>
+      </c>
+      <c r="C73">
+        <v>5</v>
+      </c>
+      <c r="D73" t="s">
+        <v>12</v>
+      </c>
+      <c r="E73" s="5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B74">
+        <v>99</v>
+      </c>
+      <c r="C74">
+        <v>5.67</v>
+      </c>
+      <c r="D74" t="s">
+        <v>12</v>
+      </c>
+      <c r="E74" s="5">
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B75">
+        <v>100</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75" t="s">
+        <v>12</v>
+      </c>
+      <c r="E75" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B73">
+      <c r="B76">
         <v>0</v>
       </c>
-      <c r="C73">
+      <c r="C76">
         <v>0</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D76" t="s">
         <v>13</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E76" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="6"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B75" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C75" s="32"/>
-      <c r="D75" s="32"/>
-      <c r="E75" s="32"/>
-    </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B79" t="s">
-        <v>86</v>
-      </c>
+      <c r="A77" s="6"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="C78" s="32"/>
+      <c r="D78" s="32"/>
+      <c r="E78" s="32"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-      <c r="B80" t="s">
-        <v>77</v>
-      </c>
-      <c r="C80" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
-      <c r="B81">
-        <v>1</v>
-      </c>
-      <c r="C81">
-        <v>8</v>
+      <c r="A80" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="2"/>
-      <c r="B82">
-        <v>2</v>
-      </c>
-      <c r="C82">
-        <v>3</v>
+      <c r="A82" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B82" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
-      <c r="B83">
-        <v>0</v>
-      </c>
-      <c r="C83">
-        <v>5</v>
+      <c r="B83" t="s">
+        <v>220</v>
+      </c>
+      <c r="C83" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C84">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -4240,96 +4543,121 @@
         <v>2</v>
       </c>
       <c r="C85">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C86">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
+      <c r="B88">
+        <v>2</v>
+      </c>
+      <c r="C88">
+        <v>5</v>
+      </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B89" t="s">
-        <v>93</v>
+      <c r="A89" s="2"/>
+      <c r="B89">
+        <v>3</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="2"/>
+      <c r="B90">
+        <v>5</v>
+      </c>
+      <c r="C90">
         <v>1</v>
       </c>
-      <c r="B90" t="s">
-        <v>87</v>
-      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="2"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="14" t="s">
+      <c r="A92" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B92" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B93" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B92" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C92" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="B93">
+      <c r="B95" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B96">
         <v>4</v>
       </c>
-      <c r="C93">
+      <c r="C96">
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B94">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B97">
         <v>1</v>
       </c>
-      <c r="C94">
+      <c r="C97">
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="B95">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B98">
         <v>2</v>
       </c>
-      <c r="C95">
+      <c r="C98">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B46:C46"/>
+  <mergeCells count="2">
+    <mergeCell ref="B47:C47"/>
     <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="D75:E75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4347,13 +4675,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4366,33 +4692,33 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -4421,7 +4747,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -4429,7 +4755,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -4442,21 +4768,21 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
         <v>40</v>
       </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" t="s">
-        <v>42</v>
-      </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -4468,12 +4794,12 @@
         <v>43042</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4485,12 +4811,12 @@
         <v>43042</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -4502,12 +4828,12 @@
         <v>43037</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -4519,532 +4845,589 @@
         <v>43037</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="C21" s="31"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
         <v>7</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>8</v>
       </c>
-      <c r="D28" t="s">
-        <v>27</v>
-      </c>
       <c r="E28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" t="s">
+        <v>199</v>
+      </c>
+      <c r="G28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>100</v>
+      </c>
+      <c r="F29" s="31">
+        <v>20</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="D30" s="11">
+        <v>-1</v>
+      </c>
+      <c r="E30" s="11">
+        <v>100</v>
+      </c>
+      <c r="F30" s="32">
+        <v>20</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="19">
+        <v>-1</v>
+      </c>
+      <c r="D31" s="19">
+        <v>8</v>
+      </c>
+      <c r="E31" s="19">
+        <v>100</v>
+      </c>
+      <c r="F31" s="19">
+        <v>20</v>
+      </c>
+      <c r="G31" s="34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="35">
+        <v>0</v>
+      </c>
+      <c r="D32" s="19">
+        <v>8</v>
+      </c>
+      <c r="E32" s="19">
+        <v>100</v>
+      </c>
+      <c r="F32" s="19">
+        <v>20</v>
+      </c>
+      <c r="G32" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="I32" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+    </row>
+    <row r="33" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="19">
+        <v>101</v>
+      </c>
+      <c r="D33" s="19">
+        <v>8</v>
+      </c>
+      <c r="E33" s="19">
+        <v>100</v>
+      </c>
+      <c r="F33" s="19">
+        <v>20</v>
+      </c>
+      <c r="G33" s="34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="19">
+        <v>10</v>
+      </c>
+      <c r="D34" s="19">
+        <v>8</v>
+      </c>
+      <c r="E34" s="19">
+        <v>100</v>
+      </c>
+      <c r="F34" s="19">
+        <v>20</v>
+      </c>
+      <c r="G34" s="34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>-1</v>
+      </c>
+      <c r="E35" s="31">
+        <v>100</v>
+      </c>
+      <c r="F35" s="31">
+        <v>20</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="11">
+        <v>10</v>
+      </c>
+      <c r="D36" s="11">
+        <v>0</v>
+      </c>
+      <c r="E36" s="11">
+        <v>100</v>
+      </c>
+      <c r="F36" s="31">
+        <v>20</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="31">
+        <v>10</v>
+      </c>
+      <c r="D37" s="31">
+        <v>101</v>
+      </c>
+      <c r="E37" s="31">
+        <v>100</v>
+      </c>
+      <c r="F37" s="31">
+        <v>20</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="11">
+        <v>10</v>
+      </c>
+      <c r="D38" s="11">
+        <v>100</v>
+      </c>
+      <c r="E38" s="11">
+        <v>100</v>
+      </c>
+      <c r="F38" s="31">
+        <v>20</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="19">
+        <v>10</v>
+      </c>
+      <c r="D39" s="19">
+        <v>8</v>
+      </c>
+      <c r="E39" s="19">
+        <v>-0.01</v>
+      </c>
+      <c r="F39" s="19">
+        <v>20</v>
+      </c>
+      <c r="G39" s="34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="F28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29">
+      <c r="B40" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="19">
         <v>10</v>
       </c>
-      <c r="C29">
+      <c r="D40" s="19">
         <v>8</v>
       </c>
-      <c r="D29">
+      <c r="E40" s="19">
+        <v>0</v>
+      </c>
+      <c r="F40" s="19">
+        <v>0</v>
+      </c>
+      <c r="G40" s="34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="19">
+        <v>10</v>
+      </c>
+      <c r="D41" s="19">
+        <v>8</v>
+      </c>
+      <c r="E41" s="19">
+        <v>1000.01</v>
+      </c>
+      <c r="F41" s="19">
+        <v>20</v>
+      </c>
+      <c r="G41" s="34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="19">
+        <v>10</v>
+      </c>
+      <c r="D42" s="19">
+        <v>8</v>
+      </c>
+      <c r="E42" s="19">
+        <v>1000</v>
+      </c>
+      <c r="F42" s="19">
+        <v>20</v>
+      </c>
+      <c r="G42" s="34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="11">
+        <v>10</v>
+      </c>
+      <c r="D43" s="11">
+        <v>8</v>
+      </c>
+      <c r="E43" s="31">
         <v>100</v>
       </c>
-      <c r="E29" s="31">
-        <v>20</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="33" t="s">
-        <v>226</v>
-      </c>
-      <c r="B30" s="19">
-        <v>-1</v>
-      </c>
-      <c r="C30" s="19">
+      <c r="F43" s="31">
+        <v>-0.01</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="31">
+        <v>10</v>
+      </c>
+      <c r="D44" s="31">
         <v>8</v>
       </c>
-      <c r="D30" s="19">
+      <c r="E44" s="31">
         <v>100</v>
       </c>
-      <c r="E30" s="19">
-        <v>20</v>
-      </c>
-      <c r="F30" s="34" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="B31" s="35">
+      <c r="F44" s="31">
         <v>0</v>
       </c>
-      <c r="C31" s="19">
+      <c r="G44" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="31">
+        <v>10</v>
+      </c>
+      <c r="D45" s="31">
         <v>8</v>
-      </c>
-      <c r="D31" s="19">
-        <v>100</v>
-      </c>
-      <c r="E31" s="19">
-        <v>20</v>
-      </c>
-      <c r="F31" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="H31" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-    </row>
-    <row r="32" spans="1:14" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
-        <v>213</v>
-      </c>
-      <c r="B32" s="19">
-        <v>101</v>
-      </c>
-      <c r="C32" s="19">
-        <v>8</v>
-      </c>
-      <c r="D32" s="19">
-        <v>100</v>
-      </c>
-      <c r="E32" s="19">
-        <v>20</v>
-      </c>
-      <c r="F32" s="34" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="B33" s="19">
-        <v>10</v>
-      </c>
-      <c r="C33" s="19">
-        <v>8</v>
-      </c>
-      <c r="D33" s="19">
-        <v>100</v>
-      </c>
-      <c r="E33" s="19">
-        <v>20</v>
-      </c>
-      <c r="F33" s="34" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="B34">
-        <v>10</v>
-      </c>
-      <c r="C34">
-        <v>-1</v>
-      </c>
-      <c r="D34" s="31">
-        <v>100</v>
-      </c>
-      <c r="E34" s="31">
-        <v>20</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="31" t="s">
-        <v>218</v>
-      </c>
-      <c r="B35" s="11">
-        <v>10</v>
-      </c>
-      <c r="C35" s="11">
-        <v>0</v>
-      </c>
-      <c r="D35" s="11">
-        <v>100</v>
-      </c>
-      <c r="E35" s="31">
-        <v>20</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="B36" s="31">
-        <v>10</v>
-      </c>
-      <c r="C36" s="31">
-        <v>101</v>
-      </c>
-      <c r="D36" s="31">
-        <v>100</v>
-      </c>
-      <c r="E36" s="31">
-        <v>20</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
-        <v>219</v>
-      </c>
-      <c r="B37" s="11">
-        <v>10</v>
-      </c>
-      <c r="C37" s="11">
-        <v>100</v>
-      </c>
-      <c r="D37" s="11">
-        <v>100</v>
-      </c>
-      <c r="E37" s="31">
-        <v>20</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="33" t="s">
-        <v>227</v>
-      </c>
-      <c r="B38" s="19">
-        <v>10</v>
-      </c>
-      <c r="C38" s="19">
-        <v>8</v>
-      </c>
-      <c r="D38" s="19">
-        <v>-0.01</v>
-      </c>
-      <c r="E38" s="19">
-        <v>20</v>
-      </c>
-      <c r="F38" s="34" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="B39" s="19">
-        <v>10</v>
-      </c>
-      <c r="C39" s="19">
-        <v>8</v>
-      </c>
-      <c r="D39" s="19">
-        <v>0</v>
-      </c>
-      <c r="E39" s="19">
-        <v>0</v>
-      </c>
-      <c r="F39" s="34" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="33" t="s">
-        <v>212</v>
-      </c>
-      <c r="B40" s="19">
-        <v>10</v>
-      </c>
-      <c r="C40" s="19">
-        <v>8</v>
-      </c>
-      <c r="D40" s="19">
-        <v>1000.01</v>
-      </c>
-      <c r="E40" s="19">
-        <v>20</v>
-      </c>
-      <c r="F40" s="34" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="B41" s="19">
-        <v>10</v>
-      </c>
-      <c r="C41" s="19">
-        <v>8</v>
-      </c>
-      <c r="D41" s="19">
-        <v>1000</v>
-      </c>
-      <c r="E41" s="19">
-        <v>20</v>
-      </c>
-      <c r="F41" s="34" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="B42" s="11">
-        <v>10</v>
-      </c>
-      <c r="C42" s="11">
-        <v>8</v>
-      </c>
-      <c r="D42" s="31">
-        <v>100</v>
-      </c>
-      <c r="E42" s="31">
-        <v>-0.01</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="B43" s="31">
-        <v>10</v>
-      </c>
-      <c r="C43" s="31">
-        <v>8</v>
-      </c>
-      <c r="D43" s="31">
-        <v>100</v>
-      </c>
-      <c r="E43" s="31">
-        <v>0</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="B44" s="31">
-        <v>10</v>
-      </c>
-      <c r="C44" s="31">
-        <v>8</v>
-      </c>
-      <c r="D44" s="31">
-        <v>100</v>
-      </c>
-      <c r="E44" s="31">
-        <v>100.01</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="B45" s="31">
-        <v>10</v>
-      </c>
-      <c r="C45" s="31">
-        <v>8</v>
-      </c>
-      <c r="D45" s="11">
-        <v>100</v>
       </c>
       <c r="E45" s="31">
         <v>100</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B47" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="32"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B49" t="s">
-        <v>38</v>
-      </c>
+      <c r="F45" s="31">
+        <v>100.01</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="31">
+        <v>10</v>
+      </c>
+      <c r="D46" s="31">
+        <v>8</v>
+      </c>
+      <c r="E46" s="11">
+        <v>100</v>
+      </c>
+      <c r="F46" s="31">
+        <v>100</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B48" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="36"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B51" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="B52" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>6</v>
       </c>
-      <c r="B55" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55" t="s">
-        <v>60</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="B56" t="s">
+        <v>32</v>
+      </c>
+      <c r="C56" t="s">
         <v>58</v>
       </c>
-      <c r="E55" t="s">
-        <v>59</v>
-      </c>
-      <c r="F55" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B56" s="13">
-        <v>43042</v>
-      </c>
-      <c r="C56" s="13">
-        <v>43034</v>
-      </c>
-      <c r="D56">
-        <v>8</v>
+      <c r="D56" t="s">
+        <v>56</v>
       </c>
       <c r="E56" t="s">
-        <v>62</v>
-      </c>
-      <c r="F56" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F56" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="B57" s="13">
         <v>43042</v>
       </c>
       <c r="C57" s="13">
-        <v>43042</v>
+        <v>43034</v>
       </c>
       <c r="D57">
         <v>8</v>
       </c>
       <c r="E57" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B58" s="13">
         <v>43042</v>
       </c>
       <c r="C58" s="13">
-        <v>43034</v>
+        <v>43042</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E58" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B59" s="13">
         <v>43042</v>
@@ -5053,46 +5436,66 @@
         <v>43034</v>
       </c>
       <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59" t="s">
+        <v>60</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="13">
+        <v>43042</v>
+      </c>
+      <c r="C60" s="13">
+        <v>43034</v>
+      </c>
+      <c r="D60">
         <v>8</v>
       </c>
-      <c r="E59" s="11"/>
-      <c r="F59" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="B60" s="13"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
       <c r="E60" s="11"/>
-      <c r="F60" s="1"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F60" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B61" s="13">
+        <v>214</v>
+      </c>
+      <c r="B61" s="13"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="13">
         <v>43042</v>
       </c>
-      <c r="C61" s="13">
+      <c r="C62" s="13">
         <v>43034</v>
       </c>
-      <c r="D61">
+      <c r="D62">
         <v>8</v>
       </c>
-      <c r="E61" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>51</v>
+      <c r="E62" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5106,12 +5509,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5122,41 +5525,49 @@
     <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="12"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" s="32" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>7</v>
       </c>
@@ -5167,7 +5578,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>100</v>
       </c>
@@ -5177,8 +5588,14 @@
       <c r="D9" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>99</v>
       </c>
@@ -5189,149 +5606,184 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
-        <v>9.5</v>
+        <v>95</v>
       </c>
       <c r="C11" s="4">
-        <v>8.5</v>
+        <v>85</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="14" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="39">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="39">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="39">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="23"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
         <v>72</v>
       </c>
-      <c r="C13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="32">
         <v>1</v>
       </c>
-      <c r="C23">
+      <c r="C25" s="32">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="32">
+        <v>2</v>
+      </c>
+      <c r="C26" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="32">
+        <v>0</v>
+      </c>
+      <c r="C27" s="32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="32">
+        <v>2</v>
+      </c>
+      <c r="C28" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="32">
+        <v>2</v>
+      </c>
+      <c r="C29" s="32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="32">
+        <v>3</v>
+      </c>
+      <c r="C30" s="32">
         <v>1</v>
       </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="32">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26">
+      <c r="C31" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="C27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>5</v>
-      </c>
-      <c r="C28">
+      <c r="B33" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>5</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
-        <v>83</v>
+      <c r="B34" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
@@ -5350,47 +5802,47 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>155</v>
-      </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
+        <v>154</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D7" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -5493,7 +5945,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -5507,7 +5959,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -5524,7 +5976,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5532,7 +5984,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5540,16 +5992,16 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="C21" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="D21" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -5568,7 +6020,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
@@ -5576,7 +6028,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -5584,18 +6036,18 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B27" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -5603,7 +6055,7 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -5611,28 +6063,28 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="B33" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B34" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B35" s="9">
         <v>43399</v>
@@ -5640,7 +6092,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B36" s="9">
         <v>43393</v>
@@ -5648,7 +6100,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B38" s="21"/>
       <c r="C38" s="21"/>
@@ -5660,10 +6112,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B41" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -5671,29 +6123,29 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B44" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="C45" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="D45" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E45" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -5712,23 +6164,23 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C49" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C50" s="8">
         <v>3578000</v>
@@ -5739,26 +6191,26 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C53" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D53" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E53" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C54">
         <v>0.8</v>
@@ -5772,7 +6224,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B56" s="21"/>
       <c r="C56" s="21"/>
@@ -5794,7 +6246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
@@ -5814,42 +6266,42 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
+        <v>154</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D6" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -5952,7 +6404,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -5966,7 +6418,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -5983,7 +6435,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5991,7 +6443,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -5999,16 +6451,16 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="C20" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="D20" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -6069,7 +6521,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
@@ -6077,10 +6529,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B29" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -6088,37 +6540,37 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B32" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C33" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D33" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="E33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F33" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C34" s="9">
         <v>42527</v>
@@ -6135,7 +6587,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="C35" s="9">
         <v>42005</v>
@@ -6152,23 +6604,23 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C38" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C39" s="8">
         <v>3578000</v>
@@ -6176,7 +6628,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="C40" s="8">
         <v>4578000</v>
@@ -6187,26 +6639,26 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C43" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D43" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E43" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C44">
         <v>0.8</v>
@@ -6220,7 +6672,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="C45">
         <v>0</v>

</xml_diff>

<commit_message>
Entrego Genere las métricas de todas las iteraciones del proyecto
</commit_message>
<xml_diff>
--- a/Especificaciones.xlsx
+++ b/Especificaciones.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13875" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13875" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Introducción" sheetId="6" r:id="rId1"/>
@@ -431,7 +431,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="265">
   <si>
     <t>Genere la métrica de puntos</t>
   </si>
@@ -850,9 +850,6 @@
     <t>Escenario</t>
   </si>
   <si>
-    <t>Genere el resumen de todas las iteraciones del proyecto</t>
-  </si>
-  <si>
     <t>que la fecha actual es "1/1/2016"</t>
   </si>
   <si>
@@ -928,9 +925,6 @@
     <t>Valor de mercado = monto nominal del saldo * (precio limpio del vector de precios / 100);</t>
   </si>
   <si>
-    <t>Valoración de las emisiones en colones</t>
-  </si>
-  <si>
     <t>se valora las emisiones</t>
   </si>
   <si>
@@ -1132,12 +1126,6 @@
     <t>Genere la valoración de una emisión en colones</t>
   </si>
   <si>
-    <t>se consulta el resumen de las iteraciones</t>
-  </si>
-  <si>
-    <t>se obtiene un resumen por cada iteracion</t>
-  </si>
-  <si>
     <t>80% 8|10</t>
   </si>
   <si>
@@ -1223,6 +1211,21 @@
   </si>
   <si>
     <t>se calcula el valor de mercado de una emisión con un &lt;monto nominal del saldo&gt;</t>
+  </si>
+  <si>
+    <t>HDA000000000003</t>
+  </si>
+  <si>
+    <t>Genere la valoración de las emisiones en colones</t>
+  </si>
+  <si>
+    <t>Genere las métricas de todas las iteraciones del proyecto</t>
+  </si>
+  <si>
+    <t>se consulta las métricas de las iteraciones</t>
+  </si>
+  <si>
+    <t>se obtiene las métricas de cada iteracion</t>
   </si>
 </sst>
 </file>
@@ -3217,8 +3220,8 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Table2431" displayName="Table2431" ref="B32:E34" totalsRowShown="0">
-  <autoFilter ref="B32:E34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Table2431" displayName="Table2431" ref="B34:E37" totalsRowShown="0">
+  <autoFilter ref="B34:E37"/>
   <tableColumns count="4">
     <tableColumn id="1" name="ISIN"/>
     <tableColumn id="2" name="Porcentaje de cobertura"/>
@@ -3230,8 +3233,8 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Table2532" displayName="Table2532" ref="B22:F24" totalsRowShown="0">
-  <autoFilter ref="B22:F24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Table2532" displayName="Table2532" ref="B22:F25" totalsRowShown="0">
+  <autoFilter ref="B22:F25"/>
   <tableColumns count="5">
     <tableColumn id="5" name="ISIN" dataDxfId="37"/>
     <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="36"/>
@@ -3244,8 +3247,8 @@
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="Table2633" displayName="Table2633" ref="B27:C29" totalsRowShown="0">
-  <autoFilter ref="B27:C29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="Table2633" displayName="Table2633" ref="B28:C31" totalsRowShown="0">
+  <autoFilter ref="B28:C31"/>
   <tableColumns count="2">
     <tableColumn id="1" name="ISIN"/>
     <tableColumn id="2" name="Monto nominal del saldo" dataCellStyle="Comma"/>
@@ -3958,7 +3961,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -4178,139 +4181,139 @@
     <row r="83" spans="1:1" s="29" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="84" spans="1:1" s="29" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="46" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="85" spans="1:1" s="29" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A85" s="40" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="11" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="29" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="29" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="29" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="29" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="11" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -4343,7 +4346,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -4353,87 +4356,87 @@
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="41" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="41" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="41" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -4473,14 +4476,14 @@
         <v>138</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3"/>
     </row>
     <row r="4" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -4497,7 +4500,7 @@
         <v>46</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C6" s="8"/>
     </row>
@@ -4506,7 +4509,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C7" s="8"/>
     </row>
@@ -4515,7 +4518,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C8" s="8"/>
     </row>
@@ -4532,10 +4535,10 @@
     <row r="11" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>33</v>
@@ -4563,12 +4566,12 @@
         <v>138</v>
       </c>
       <c r="B14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4581,10 +4584,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4592,7 +4595,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4600,7 +4603,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4616,18 +4619,18 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" t="s">
         <v>144</v>
       </c>
-      <c r="E23" t="s">
-        <v>145</v>
-      </c>
       <c r="F23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C24" s="8">
         <v>42370</v>
@@ -4644,7 +4647,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C25" s="8">
         <v>42370</v>
@@ -4661,7 +4664,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C26" s="8">
         <v>42370</v>
@@ -4691,13 +4694,13 @@
         <v>138</v>
       </c>
       <c r="B29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -4712,10 +4715,10 @@
         <v>33</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -4752,7 +4755,7 @@
     </row>
     <row r="37" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -4883,7 +4886,7 @@
         <v>138</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C50" s="33"/>
     </row>
@@ -4894,7 +4897,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -4952,7 +4955,7 @@
         <v>95</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -4969,7 +4972,7 @@
         <v>90</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -5038,7 +5041,7 @@
     </row>
     <row r="67" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -5076,7 +5079,7 @@
         <v>27</v>
       </c>
       <c r="F73" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -5212,7 +5215,7 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -5356,7 +5359,7 @@
         <v>138</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C21" s="28"/>
     </row>
@@ -5368,7 +5371,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -5404,7 +5407,7 @@
         <v>26</v>
       </c>
       <c r="H28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I28" t="s">
         <v>43</v>
@@ -5438,7 +5441,7 @@
     </row>
     <row r="30" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C30" s="39" t="s">
         <v>13</v>
@@ -5464,7 +5467,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B31" s="30" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>12</v>
@@ -5490,7 +5493,7 @@
     </row>
     <row r="32" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>12</v>
@@ -5514,7 +5517,7 @@
         <v>41</v>
       </c>
       <c r="J32" s="20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
@@ -5525,7 +5528,7 @@
     </row>
     <row r="33" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>12</v>
@@ -5551,7 +5554,7 @@
     </row>
     <row r="34" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>12</v>
@@ -5577,7 +5580,7 @@
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="28" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>12</v>
@@ -5603,7 +5606,7 @@
     </row>
     <row r="36" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>12</v>
@@ -5629,7 +5632,7 @@
     </row>
     <row r="37" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="28" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>12</v>
@@ -5655,7 +5658,7 @@
     </row>
     <row r="38" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>12</v>
@@ -5681,7 +5684,7 @@
     </row>
     <row r="39" spans="2:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>12</v>
@@ -5707,7 +5710,7 @@
     </row>
     <row r="40" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="30" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>12</v>
@@ -5733,7 +5736,7 @@
     </row>
     <row r="41" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>12</v>
@@ -5759,7 +5762,7 @@
     </row>
     <row r="42" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>12</v>
@@ -5785,7 +5788,7 @@
     </row>
     <row r="43" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>12</v>
@@ -5811,7 +5814,7 @@
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>12</v>
@@ -5837,7 +5840,7 @@
     </row>
     <row r="45" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>12</v>
@@ -5863,7 +5866,7 @@
     </row>
     <row r="46" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>12</v>
@@ -5889,7 +5892,7 @@
     </row>
     <row r="47" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>12</v>
@@ -6051,7 +6054,7 @@
     </row>
     <row r="62" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C62" s="12"/>
       <c r="D62" s="10"/>
@@ -6123,7 +6126,7 @@
         <v>138</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -6131,7 +6134,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -6150,7 +6153,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6175,7 +6178,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
@@ -6208,13 +6211,13 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6248,8 +6251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6267,7 +6270,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B1" s="11"/>
     </row>
@@ -6338,7 +6341,7 @@
     </row>
     <row r="14" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
@@ -6353,7 +6356,7 @@
         <v>138</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -6387,7 +6390,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -6464,7 +6467,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -6495,7 +6498,7 @@
         <v>43028</v>
       </c>
       <c r="E25" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F25" s="1">
         <v>0.05</v>
@@ -6506,7 +6509,7 @@
         <v>138</v>
       </c>
       <c r="B28" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -6514,37 +6517,37 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" t="s">
         <v>141</v>
-      </c>
-      <c r="B31" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C32" t="s">
+        <v>143</v>
+      </c>
+      <c r="D32" t="s">
         <v>144</v>
-      </c>
-      <c r="D32" t="s">
-        <v>145</v>
       </c>
       <c r="E32" t="s">
         <v>34</v>
       </c>
       <c r="F32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" s="29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C33" s="8">
         <v>42527</v>
@@ -6564,20 +6567,20 @@
         <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C37" s="7">
         <v>3578000</v>
@@ -6588,12 +6591,12 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C40" t="s">
         <v>34</v>
@@ -6607,7 +6610,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C41">
         <v>0.8</v>
@@ -6621,7 +6624,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B43" s="20"/>
       <c r="C43" s="20"/>
@@ -6642,10 +6645,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6664,7 +6667,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B1" s="11"/>
     </row>
@@ -6674,7 +6677,7 @@
         <v>138</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>139</v>
+        <v>262</v>
       </c>
       <c r="C3" s="33"/>
       <c r="D3" s="33"/>
@@ -6685,7 +6688,7 @@
         <v>67</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6693,10 +6696,10 @@
         <v>38</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E6" s="34" t="s">
         <v>9</v>
@@ -6797,8 +6800,12 @@
       <c r="H9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6806,7 +6813,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>233</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6814,7 +6821,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>234</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6845,7 +6852,7 @@
         <v>43028</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F14" s="1">
         <v>0.05</v>
@@ -6891,7 +6898,7 @@
         <v>138</v>
       </c>
       <c r="B18" t="s">
-        <v>165</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -6899,37 +6906,37 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B21" t="s">
         <v>141</v>
-      </c>
-      <c r="B21" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C22" t="s">
+        <v>143</v>
+      </c>
+      <c r="D22" t="s">
         <v>144</v>
-      </c>
-      <c r="D22" t="s">
-        <v>145</v>
       </c>
       <c r="E22" t="s">
         <v>34</v>
       </c>
       <c r="F22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C23" s="8">
         <v>42527</v>
@@ -6946,10 +6953,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C24" s="8">
-        <v>42005</v>
+        <v>42370</v>
       </c>
       <c r="D24">
         <v>14</v>
@@ -6961,86 +6968,127 @@
         <v>800</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="25" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C25" s="8">
+        <v>42005</v>
+      </c>
+      <c r="D25" s="29">
+        <v>14</v>
+      </c>
+      <c r="E25" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="F25" s="29">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B26" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>147</v>
-      </c>
-      <c r="C27" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>146</v>
+      </c>
+      <c r="C28" t="s">
         <v>148</v>
-      </c>
-      <c r="C28" s="7">
-        <v>3578000</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="C29" s="7">
+        <v>3578000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C30" s="7">
         <v>4578000</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C31" s="7">
+        <v>6576000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B31" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="B33" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>147</v>
       </c>
-      <c r="C32" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>148</v>
-      </c>
-      <c r="C33">
+      <c r="C35">
         <v>0.8</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D35" s="7">
         <v>2862400</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E35" s="7">
         <v>2289920</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>167</v>
-      </c>
-      <c r="C34">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>165</v>
+      </c>
+      <c r="C36">
         <v>0</v>
       </c>
-      <c r="D34" s="7">
-        <f>+C29*(F24/100)</f>
+      <c r="D36" s="7">
+        <f>+C30*(F24/100)</f>
         <v>36624000</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E36" s="7">
+        <f>Table2431[[#This Row],[Valor de mercado]]*Table2431[[#This Row],[Porcentaje de cobertura]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C37" s="29">
+        <v>0</v>
+      </c>
+      <c r="D37" s="7">
+        <f>+C31*(F25/100)</f>
+        <v>52608000</v>
+      </c>
+      <c r="E37" s="7">
         <f>Table2431[[#This Row],[Valor de mercado]]*Table2431[[#This Row],[Porcentaje de cobertura]]</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Entrego Genere la valoración de las emisiones en colones
</commit_message>
<xml_diff>
--- a/Especificaciones.xlsx
+++ b/Especificaciones.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13875" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13875"/>
   </bookViews>
   <sheets>
     <sheet name="Introducción" sheetId="6" r:id="rId1"/>
@@ -3652,8 +3652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6647,8 +6647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mejoras a las especificaciones y ejemplos.
</commit_message>
<xml_diff>
--- a/Especificaciones.xlsx
+++ b/Especificaciones.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13875"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13875" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introducción" sheetId="6" r:id="rId1"/>
@@ -751,18 +751,12 @@
     <t>una cuenta con saldo &lt;saldo inicial&gt;</t>
   </si>
   <si>
-    <t>el saldo es de  &lt;nuevo saldo&gt; colones</t>
-  </si>
-  <si>
     <t>Saldo inicial</t>
   </si>
   <si>
     <t>Monto a retirar</t>
   </si>
   <si>
-    <t>Nuevo Saldo</t>
-  </si>
-  <si>
     <t>Se puede retirar fondos suficientes</t>
   </si>
   <si>
@@ -910,9 +904,6 @@
     <t>Porcentaje de cobertura revisado</t>
   </si>
   <si>
-    <t>Además, siempre utilice las palabras del negocio, no palabras técnica o abreviaturas que no sean comunes.</t>
-  </si>
-  <si>
     <t>Cálculo del aporte de garantía</t>
   </si>
   <si>
@@ -1226,6 +1217,15 @@
   </si>
   <si>
     <t>se obtiene las métricas de cada iteracion</t>
+  </si>
+  <si>
+    <t>Nuevosaldo</t>
+  </si>
+  <si>
+    <t>el saldo es de &lt;nuevo saldo&gt; colones</t>
+  </si>
+  <si>
+    <t>Además, siempre utilice las palabras del negocio, no palabras técnicas o abreviaturas que no sean comunes.</t>
   </si>
 </sst>
 </file>
@@ -1526,7 +1526,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="8" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="7"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1545,6 +1544,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="11" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="20% - Accent1" xfId="8" builtinId="30"/>
@@ -1561,248 +1561,6 @@
     <cellStyle name="Percent" xfId="11" builtinId="5"/>
   </cellStyles>
   <dxfs count="78">
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1895,7 +1653,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1906,46 +1663,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2044,6 +1761,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2086,17 +1804,80 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="4"/>
         </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
+        <right/>
         <top style="thin">
           <color theme="4"/>
         </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -2195,6 +1976,61 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -2253,17 +2089,51 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
         <right/>
         <top style="thin">
           <color theme="4"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -2307,27 +2177,10 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -2345,6 +2198,34 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2401,13 +2282,27 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2564,6 +2459,23 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -2787,6 +2699,60 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="4"/>
@@ -2845,6 +2811,40 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
     </dxf>
     <dxf>
@@ -3042,7 +3042,7 @@
     <tableColumn id="1" name="Ejemplo"/>
     <tableColumn id="2" name="Saldo inicial"/>
     <tableColumn id="3" name="Monto a retirar"/>
-    <tableColumn id="4" name="Nuevo Saldo"/>
+    <tableColumn id="4" name="Nuevosaldo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3052,7 +3052,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="B15:F19" totalsRowShown="0">
   <autoFilter ref="B15:F19"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="52"/>
+    <tableColumn id="1" name="Ejemplo" dataDxfId="48"/>
     <tableColumn id="2" name="Numero"/>
     <tableColumn id="3" name="Fecha inicial"/>
     <tableColumn id="4" name="Fecha final"/>
@@ -3066,8 +3066,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="B6:C8" totalsRowShown="0">
   <autoFilter ref="B6:C8"/>
   <tableColumns count="2">
-    <tableColumn id="2" name="Fecha de inicio" dataDxfId="51"/>
-    <tableColumn id="3" name="Fecha final" dataDxfId="50"/>
+    <tableColumn id="2" name="Fecha de inicio" dataDxfId="47"/>
+    <tableColumn id="3" name="Fecha final" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3077,14 +3077,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table168" displayName="Table168" ref="B28:I47" totalsRowShown="0">
   <autoFilter ref="B28:I47"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="49"/>
-    <tableColumn id="7" name="Hay informacion de puntos disponible" dataDxfId="35"/>
+    <tableColumn id="1" name="Ejemplo" dataDxfId="45"/>
+    <tableColumn id="7" name="Hay informacion de puntos disponible" dataDxfId="44"/>
     <tableColumn id="2" name="Puntos planificados" dataCellStyle="Normal"/>
     <tableColumn id="3" name="Puntos terminados" dataCellStyle="Normal"/>
     <tableColumn id="8" name="Hay informacion de dias disponible"/>
     <tableColumn id="4" name="Capacidad del equipo" dataCellStyle="Normal"/>
     <tableColumn id="5" name="Días no efectivos"/>
-    <tableColumn id="6" name="Es válida o no" dataDxfId="48"/>
+    <tableColumn id="6" name="Es válida o no" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3094,34 +3094,34 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1689" displayName="Table1689" ref="B57:G63" totalsRowShown="0">
   <autoFilter ref="B57:G63"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="47"/>
-    <tableColumn id="7" name="Fecha actual" dataDxfId="46"/>
+    <tableColumn id="1" name="Ejemplo" dataDxfId="42"/>
+    <tableColumn id="7" name="Fecha actual" dataDxfId="41"/>
     <tableColumn id="2" name="Fecha de reporte" dataCellStyle="Normal"/>
     <tableColumn id="3" name="Total de incidentes" dataCellStyle="Normal"/>
     <tableColumn id="4" name="Descripción" dataCellStyle="Normal"/>
-    <tableColumn id="6" name="Es válida o no" dataDxfId="45"/>
+    <tableColumn id="6" name="Es válida o no" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="B8:D11" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" tableBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="B8:D11" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="37">
   <autoFilter ref="B8:D11"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Puntos planificados" dataDxfId="41"/>
-    <tableColumn id="2" name="Puntos terminados" dataDxfId="40"/>
-    <tableColumn id="3" name="Hay informacion de puntos disponible" dataDxfId="39"/>
+    <tableColumn id="1" name="Puntos planificados" dataDxfId="36"/>
+    <tableColumn id="2" name="Puntos terminados" dataDxfId="35"/>
+    <tableColumn id="3" name="Hay informacion de puntos disponible" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table5" displayName="Table5" ref="B14:B17" totalsRowShown="0" headerRowDxfId="31" dataDxfId="32" tableBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table5" displayName="Table5" ref="B14:B17" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" tableBorderDxfId="31">
   <autoFilter ref="B14:B17"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Métricas de puntos" dataDxfId="33"/>
+    <tableColumn id="1" name="Métricas de puntos" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3132,8 +3132,8 @@
   <autoFilter ref="B24:F25"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Iteración"/>
-    <tableColumn id="2" name="Fecha inicial" dataDxfId="6"/>
-    <tableColumn id="6" name="Fecha final" dataDxfId="5"/>
+    <tableColumn id="2" name="Fecha inicial" dataDxfId="29"/>
+    <tableColumn id="6" name="Fecha final" dataDxfId="28"/>
     <tableColumn id="4" name="Métrica de puntos"/>
     <tableColumn id="5" name="Métrica de tiempo no efectivo"/>
   </tableColumns>
@@ -3169,8 +3169,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Table25" displayName="Table25" ref="B32:F33" totalsRowShown="0">
   <autoFilter ref="B32:F33"/>
   <tableColumns count="5">
-    <tableColumn id="5" name="ISIN" dataDxfId="0"/>
-    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="38"/>
+    <tableColumn id="5" name="ISIN" dataDxfId="27"/>
+    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="26"/>
     <tableColumn id="2" name="Dias minimos al vencimiento del emisor"/>
     <tableColumn id="3" name="Porcentaje de cobertura"/>
     <tableColumn id="4" name="Precio limpio del vector de precios"/>
@@ -3202,18 +3202,18 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table22" displayName="Table22" ref="B20:J21" totalsRowShown="0" headerRowDxfId="15" dataDxfId="16" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table22" displayName="Table22" ref="B20:J21" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" tableBorderDxfId="23">
   <autoFilter ref="B20:J21"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Numero" dataDxfId="7"/>
-    <tableColumn id="2" name="Fecha inicial" dataDxfId="8"/>
-    <tableColumn id="3" name="Fecha final" dataDxfId="21"/>
-    <tableColumn id="10" name="Hay informacion de puntos disponible" dataDxfId="14"/>
-    <tableColumn id="4" name="Puntos planificados" dataDxfId="20"/>
-    <tableColumn id="5" name="Puntos terminados" dataDxfId="19"/>
-    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="13"/>
-    <tableColumn id="7" name="Capacidad del equipo" dataDxfId="18"/>
-    <tableColumn id="8" name="Dias no efectivos" dataDxfId="17"/>
+    <tableColumn id="1" name="Numero" dataDxfId="22"/>
+    <tableColumn id="2" name="Fecha inicial" dataDxfId="21"/>
+    <tableColumn id="3" name="Fecha final" dataDxfId="20"/>
+    <tableColumn id="10" name="Hay informacion de puntos disponible" dataDxfId="19"/>
+    <tableColumn id="4" name="Puntos planificados" dataDxfId="18"/>
+    <tableColumn id="5" name="Puntos terminados" dataDxfId="17"/>
+    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="16"/>
+    <tableColumn id="7" name="Capacidad del equipo" dataDxfId="15"/>
+    <tableColumn id="8" name="Dias no efectivos" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3236,8 +3236,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Table2532" displayName="Table2532" ref="B22:F25" totalsRowShown="0">
   <autoFilter ref="B22:F25"/>
   <tableColumns count="5">
-    <tableColumn id="5" name="ISIN" dataDxfId="37"/>
-    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="36"/>
+    <tableColumn id="5" name="ISIN" dataDxfId="13"/>
+    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="12"/>
     <tableColumn id="2" name="Dias minimos al vencimiento del emisor"/>
     <tableColumn id="3" name="Porcentaje de cobertura"/>
     <tableColumn id="4" name="Precio limpio del vector de precios"/>
@@ -3258,18 +3258,18 @@
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table1819" displayName="Table1819" ref="B6:J9" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table1819" displayName="Table1819" ref="B6:J9" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="B6:J9"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Numero"/>
-    <tableColumn id="2" name="fecha inicial" dataDxfId="28"/>
-    <tableColumn id="3" name="fecha final" dataDxfId="27"/>
-    <tableColumn id="10" name="Hay informacion de puntos disponible" dataDxfId="10"/>
-    <tableColumn id="4" name="Puntos planificados" dataDxfId="26"/>
-    <tableColumn id="5" name="Puntos terminados" dataDxfId="25"/>
-    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="9"/>
-    <tableColumn id="7" name="Capacidad del equipo" dataDxfId="24"/>
-    <tableColumn id="8" name="Dias no efectivos" dataDxfId="23"/>
+    <tableColumn id="2" name="fecha inicial" dataDxfId="9"/>
+    <tableColumn id="3" name="fecha final" dataDxfId="8"/>
+    <tableColumn id="10" name="Hay informacion de puntos disponible" dataDxfId="7"/>
+    <tableColumn id="4" name="Puntos planificados" dataDxfId="6"/>
+    <tableColumn id="5" name="Puntos terminados" dataDxfId="5"/>
+    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="4"/>
+    <tableColumn id="7" name="Capacidad del equipo" dataDxfId="3"/>
+    <tableColumn id="8" name="Dias no efectivos" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3280,8 +3280,8 @@
   <autoFilter ref="B13:F16"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Iteración"/>
-    <tableColumn id="2" name="Fecha inicial" dataDxfId="12"/>
-    <tableColumn id="6" name="Fecha final" dataDxfId="11"/>
+    <tableColumn id="2" name="Fecha inicial" dataDxfId="1"/>
+    <tableColumn id="6" name="Fecha final" dataDxfId="0"/>
     <tableColumn id="4" name="Métrica de puntos"/>
     <tableColumn id="5" name="Métrica de tiempo no efectivo"/>
   </tableColumns>
@@ -3320,7 +3320,7 @@
   <autoFilter ref="B58:F63"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Ejemplo" dataDxfId="67"/>
-    <tableColumn id="6" name="Hay informacion de puntos disponible" dataDxfId="4"/>
+    <tableColumn id="6" name="Hay informacion de puntos disponible" dataDxfId="66"/>
     <tableColumn id="2" name="Puntos planificados"/>
     <tableColumn id="3" name="Puntos terminados"/>
     <tableColumn id="5" name="Métrica de puntos"/>
@@ -3333,8 +3333,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B73:F77" totalsRowShown="0">
   <autoFilter ref="B73:F77"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Ejemplo" dataDxfId="66"/>
-    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="3"/>
+    <tableColumn id="1" name="Ejemplo" dataDxfId="65"/>
+    <tableColumn id="6" name="Hay informacion de dias disponible" dataDxfId="64"/>
     <tableColumn id="2" name="Capacidad del equipo"/>
     <tableColumn id="3" name="Dias no efectivos"/>
     <tableColumn id="5" name="Tiempo no efectivo"/>
@@ -3347,9 +3347,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Table27" displayName="Table27" ref="B23:F26" totalsRowShown="0">
   <autoFilter ref="B23:F26"/>
   <tableColumns count="5">
-    <tableColumn id="5" name="Ejemplo" dataDxfId="65"/>
-    <tableColumn id="4" name="Fecha actual" dataDxfId="64"/>
-    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="63"/>
+    <tableColumn id="5" name="Ejemplo" dataDxfId="63"/>
+    <tableColumn id="4" name="Fecha actual" dataDxfId="62"/>
+    <tableColumn id="1" name="Fecha de vencimiento del valor oficial" dataDxfId="61"/>
     <tableColumn id="2" name="Dias minimos al vencimiento del emisor"/>
     <tableColumn id="3" name="Porcentaje de cobertura revisado"/>
   </tableColumns>
@@ -3358,12 +3358,12 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Table28" displayName="Table28" ref="B11:D12" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" tableBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Table28" displayName="Table28" ref="B11:D12" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" tableBorderDxfId="58">
   <autoFilter ref="B11:D12"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Precio limpio del vector de precios" dataDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="2" name="Monto nominal del saldo" dataDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="Valor de mercado" dataDxfId="59" dataCellStyle="Comma">
+    <tableColumn id="1" name="Precio limpio del vector de precios" dataDxfId="57" dataCellStyle="Comma"/>
+    <tableColumn id="2" name="Monto nominal del saldo" dataDxfId="56" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="Valor de mercado" dataDxfId="55" dataCellStyle="Comma">
       <calculatedColumnFormula>+Table28[Precio limpio del vector de precios]*(Table28[Monto nominal del saldo]/100)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3372,14 +3372,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Table2830" displayName="Table2830" ref="B32:D33" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57" tableBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Table2830" displayName="Table2830" ref="B32:D33" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53" tableBorderDxfId="52">
   <autoFilter ref="B32:D33"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Valor de mercado" dataDxfId="55" dataCellStyle="Comma">
+    <tableColumn id="1" name="Valor de mercado" dataDxfId="51" dataCellStyle="Comma">
       <calculatedColumnFormula>+Table28[Precio limpio del vector de precios]*(Table28[Monto nominal del saldo]/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Porcentaje de cobertura revisado" dataDxfId="54"/>
-    <tableColumn id="3" name="Aporte de garantía" dataDxfId="53" dataCellStyle="Comma">
+    <tableColumn id="2" name="Porcentaje de cobertura revisado" dataDxfId="50"/>
+    <tableColumn id="3" name="Aporte de garantía" dataDxfId="49" dataCellStyle="Comma">
       <calculatedColumnFormula>+Table2830[Valor de mercado]*Table2830[Porcentaje de cobertura revisado]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3652,8 +3652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84:A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3873,7 +3873,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>106</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3886,18 +3886,18 @@
         <v>6</v>
       </c>
       <c r="C38" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" t="s">
         <v>107</v>
       </c>
-      <c r="D38" t="s">
-        <v>108</v>
-      </c>
       <c r="E38" t="s">
-        <v>109</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C39">
         <v>1000</v>
@@ -3911,7 +3911,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C40">
         <v>1000</v>
@@ -3925,7 +3925,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C41">
         <v>1000</v>
@@ -3939,7 +3939,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C42">
         <v>1000</v>
@@ -3953,48 +3953,48 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B44" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>159</v>
+        <v>264</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4142,178 +4142,178 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B74" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="83" spans="1:1" s="29" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="84" spans="1:1" s="29" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="46" t="s">
-        <v>253</v>
+      <c r="A84" s="45" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="85" spans="1:1" s="29" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="40" t="s">
-        <v>254</v>
+      <c r="A85" s="39" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="11" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="29" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="29" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="29" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="29" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="11" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -4335,8 +4335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4346,7 +4346,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -4356,87 +4356,87 @@
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
-        <v>200</v>
+      <c r="A8" s="40" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
-        <v>201</v>
+      <c r="A9" s="40" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
-        <v>202</v>
+      <c r="A13" s="40" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
-        <v>203</v>
+      <c r="A14" s="40" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
-        <v>204</v>
+      <c r="A15" s="40" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -4473,17 +4473,17 @@
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3"/>
     </row>
     <row r="4" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -4496,49 +4496,49 @@
       <c r="D5"/>
     </row>
     <row r="6" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="46" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="46" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="46"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="46" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>33</v>
@@ -4563,15 +4563,15 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4584,10 +4584,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4595,7 +4595,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4603,7 +4603,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4619,18 +4619,18 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C24" s="8">
         <v>42370</v>
@@ -4647,7 +4647,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C25" s="8">
         <v>42370</v>
@@ -4664,7 +4664,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C26" s="8">
         <v>42370</v>
@@ -4691,16 +4691,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B29" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -4715,10 +4715,10 @@
         <v>33</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -4741,12 +4741,12 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B35" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C35" s="33"/>
+      <c r="C35" s="47"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
@@ -4755,7 +4755,7 @@
     </row>
     <row r="37" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -4883,12 +4883,12 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B50" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="C50" s="33"/>
+        <v>136</v>
+      </c>
+      <c r="B50" s="47" t="s">
+        <v>185</v>
+      </c>
+      <c r="C50" s="47"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
@@ -4897,7 +4897,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -4955,7 +4955,7 @@
         <v>95</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -4972,7 +4972,7 @@
         <v>90</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -5028,7 +5028,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B65" t="s">
         <v>25</v>
@@ -5041,7 +5041,7 @@
     </row>
     <row r="67" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -5079,7 +5079,7 @@
         <v>27</v>
       </c>
       <c r="F73" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -5204,7 +5204,7 @@
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>37</v>
@@ -5215,7 +5215,7 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -5356,10 +5356,10 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C21" s="28"/>
     </row>
@@ -5371,7 +5371,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -5407,7 +5407,7 @@
         <v>26</v>
       </c>
       <c r="H28" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I28" t="s">
         <v>43</v>
@@ -5441,9 +5441,9 @@
     </row>
     <row r="30" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C30" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="C30" s="38" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="10">
@@ -5467,7 +5467,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B31" s="30" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>12</v>
@@ -5493,7 +5493,7 @@
     </row>
     <row r="32" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="18" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>12</v>
@@ -5517,7 +5517,7 @@
         <v>41</v>
       </c>
       <c r="J32" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
@@ -5528,7 +5528,7 @@
     </row>
     <row r="33" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>12</v>
@@ -5554,7 +5554,7 @@
     </row>
     <row r="34" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>12</v>
@@ -5580,7 +5580,7 @@
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="28" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>12</v>
@@ -5606,7 +5606,7 @@
     </row>
     <row r="36" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="28" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>12</v>
@@ -5632,7 +5632,7 @@
     </row>
     <row r="37" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="28" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>12</v>
@@ -5658,7 +5658,7 @@
     </row>
     <row r="38" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="28" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>12</v>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="39" spans="2:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>12</v>
@@ -5710,7 +5710,7 @@
     </row>
     <row r="40" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="30" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>12</v>
@@ -5736,7 +5736,7 @@
     </row>
     <row r="41" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="18" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>12</v>
@@ -5762,7 +5762,7 @@
     </row>
     <row r="42" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="30" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>12</v>
@@ -5788,7 +5788,7 @@
     </row>
     <row r="43" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="18" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>12</v>
@@ -5814,7 +5814,7 @@
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>12</v>
@@ -5840,7 +5840,7 @@
     </row>
     <row r="45" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>12</v>
@@ -5866,7 +5866,7 @@
     </row>
     <row r="46" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>12</v>
@@ -5892,7 +5892,7 @@
     </row>
     <row r="47" spans="2:9" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>12</v>
@@ -5918,12 +5918,12 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B49" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="33"/>
+      <c r="C49" s="47"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
@@ -6054,7 +6054,7 @@
     </row>
     <row r="62" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C62" s="12"/>
       <c r="D62" s="10"/>
@@ -6123,10 +6123,10 @@
     <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -6134,7 +6134,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -6153,7 +6153,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6178,7 +6178,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
@@ -6211,29 +6211,29 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="42">
+      <c r="B15" s="41">
         <v>0.95</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="42">
+      <c r="B16" s="41">
         <v>0.91</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="42">
+      <c r="B17" s="41">
         <v>0.89</v>
       </c>
     </row>
@@ -6270,17 +6270,17 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -6288,7 +6288,7 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -6296,7 +6296,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -6304,23 +6304,23 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -6333,7 +6333,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B12" s="8">
         <v>43393</v>
@@ -6341,7 +6341,7 @@
     </row>
     <row r="14" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
@@ -6353,10 +6353,10 @@
     </row>
     <row r="16" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -6390,7 +6390,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -6426,10 +6426,10 @@
       <c r="B21" s="4">
         <v>1</v>
       </c>
-      <c r="C21" s="35">
+      <c r="C21" s="34">
         <v>43024</v>
       </c>
-      <c r="D21" s="36">
+      <c r="D21" s="35">
         <v>43028</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -6452,9 +6452,9 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
@@ -6467,7 +6467,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -6491,14 +6491,14 @@
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25" s="35">
+      <c r="C25" s="34">
         <v>43024</v>
       </c>
-      <c r="D25" s="36">
+      <c r="D25" s="35">
         <v>43028</v>
       </c>
       <c r="E25" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F25" s="1">
         <v>0.05</v>
@@ -6506,10 +6506,10 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B28" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -6517,37 +6517,37 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B31" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C32" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D32" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E32" t="s">
         <v>34</v>
       </c>
       <c r="F32" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" s="29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C33" s="8">
         <v>42527</v>
@@ -6567,20 +6567,20 @@
         <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36" t="s">
         <v>146</v>
-      </c>
-      <c r="C36" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C37" s="7">
         <v>3578000</v>
@@ -6591,12 +6591,12 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C40" t="s">
         <v>34</v>
@@ -6610,7 +6610,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C41">
         <v>0.8</v>
@@ -6624,7 +6624,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B43" s="20"/>
       <c r="C43" s="20"/>
@@ -6667,28 +6667,28 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>262</v>
-      </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
+        <v>136</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
     </row>
     <row r="5" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6696,27 +6696,27 @@
         <v>38</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>218</v>
-      </c>
-      <c r="E6" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="E6" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="34" t="s">
+      <c r="G6" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="34" t="s">
+      <c r="H6" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="34" t="s">
+      <c r="J6" s="33" t="s">
         <v>27</v>
       </c>
     </row>
@@ -6724,10 +6724,10 @@
       <c r="B7" s="5">
         <v>1</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="34">
         <v>43024</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="35">
         <v>43028</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -6753,10 +6753,10 @@
       <c r="B8" s="29">
         <v>2</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="36">
         <v>43031</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="37">
         <v>43035</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -6782,10 +6782,10 @@
       <c r="B9" s="29">
         <v>3</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="34">
         <v>43038</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="35">
         <v>43042</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -6813,7 +6813,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6821,7 +6821,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -6845,14 +6845,14 @@
       <c r="B14" s="29">
         <v>1</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="34">
         <v>43024</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="35">
         <v>43028</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F14" s="1">
         <v>0.05</v>
@@ -6862,16 +6862,16 @@
       <c r="B15" s="29">
         <v>2</v>
       </c>
-      <c r="C15" s="37">
+      <c r="C15" s="36">
         <v>43031</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D15" s="37">
         <v>43035</v>
       </c>
       <c r="E15" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="45">
+      <c r="F15" s="44">
         <f>10/35</f>
         <v>0.2857142857142857</v>
       </c>
@@ -6880,10 +6880,10 @@
       <c r="B16">
         <v>3</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="34">
         <v>43038</v>
       </c>
-      <c r="D16" s="36">
+      <c r="D16" s="35">
         <v>43042</v>
       </c>
       <c r="E16" s="29" t="s">
@@ -6895,10 +6895,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B18" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -6906,37 +6906,37 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E22" t="s">
         <v>34</v>
       </c>
       <c r="F22" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C23" s="8">
         <v>42527</v>
@@ -6953,7 +6953,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C24" s="8">
         <v>42370</v>
@@ -6970,7 +6970,7 @@
     </row>
     <row r="25" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C25" s="8">
         <v>42005</v>
@@ -6990,20 +6990,20 @@
         <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" t="s">
         <v>146</v>
-      </c>
-      <c r="C28" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C29" s="7">
         <v>3578000</v>
@@ -7011,7 +7011,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C30" s="7">
         <v>4578000</v>
@@ -7019,7 +7019,7 @@
     </row>
     <row r="31" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C31" s="7">
         <v>6576000</v>
@@ -7030,12 +7030,12 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C34" t="s">
         <v>34</v>
@@ -7049,7 +7049,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C35">
         <v>0.8</v>
@@ -7063,7 +7063,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -7079,7 +7079,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C37" s="29">
         <v>0</v>

</xml_diff>